<commit_message>
change excel and ekasui templates
https://bt.abisoft.spb.ru/view.php?id=935
</commit_message>
<xml_diff>
--- a/ПОКИЛОМЕТРОВАЯ ВЕДОМОСТЬ ОТСТУПЛЕНИЙ.xlsx
+++ b/ПОКИЛОМЕТРОВАЯ ВЕДОМОСТЬ ОТСТУПЛЕНИЙ.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Дата, номер версии и производитель программного обеспечения.</t>
   </si>
@@ -25,15 +25,9 @@
     <t>Мод. и ном. диагн. ср-ва. :</t>
   </si>
   <si>
-    <t xml:space="preserve">$FORMED$ </t>
-  </si>
-  <si>
     <t>Дорога, Дистанция :</t>
   </si>
   <si>
-    <t>$RAILWAY$ ЖД, ПЧ-_______</t>
-  </si>
-  <si>
     <t xml:space="preserve">Дата, тип проверки : </t>
   </si>
   <si>
@@ -92,6 +86,15 @@
   </si>
   <si>
     <t>$REPORT_DATE$</t>
+  </si>
+  <si>
+    <t>$CARID$</t>
+  </si>
+  <si>
+    <t>$SITEID$ ЖД, ПЧ-_______</t>
+  </si>
+  <si>
+    <t>$CURRENT_OPERATOR$</t>
   </si>
 </sst>
 </file>
@@ -407,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -422,64 +425,17 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -493,12 +449,18 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -508,20 +470,62 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -829,61 +833,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -891,36 +895,36 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="25"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
+      <c r="F4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="25"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="36"/>
+      <c r="F5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="10"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -929,14 +933,16 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -946,8 +952,8 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -961,98 +967,98 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="33" t="s">
+      <c r="L8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="14" t="s">
+      <c r="M8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="16" t="s">
+    </row>
+    <row r="9" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="F9" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="K9" s="19"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="27"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="20"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="23"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="30"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1064,12 +1070,12 @@
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1081,12 +1087,12 @@
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
+      <c r="A14" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1099,6 +1105,29 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A11:M11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="K1:M1"/>
@@ -1106,29 +1135,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A11:M11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="K8:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>